<commit_message>
correction projectSource => dateModified
</commit_message>
<xml_diff>
--- a/Metadata_field_description.xlsx
+++ b/Metadata_field_description.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumniumonsac-my.sharepoint.com/personal/535606_umons_ac_be/Documents/PRIVE/UMONS/DOCTORAT/SAFEGUARD/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://alumniumonsac-my.sharepoint.com/personal/535606_umons_ac_be/Documents/PRIVE/UMONS/DOCTORAT/SAFEGUARD/SafeguardDataPaper-R/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="13_ncr:1_{C20A52EC-5834-485A-9ADB-5C7FFCEC3E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{553B359B-C6DF-402C-8387-116F762498BD}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{C20A52EC-5834-485A-9ADB-5C7FFCEC3E38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FAF1AA78-72E2-4A25-85F0-04F537766BA7}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{276831B9-4609-4F47-9D46-60B1DDBE5E9E}"/>
+    <workbookView xWindow="11100" yWindow="2220" windowWidth="27132" windowHeight="12168" xr2:uid="{276831B9-4609-4F47-9D46-60B1DDBE5E9E}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata_description" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
     <t>projectSource</t>
   </si>
   <si>
-    <t>projectUpdate</t>
-  </si>
-  <si>
     <t>datasetName</t>
   </si>
   <si>
@@ -366,6 +363,9 @@
   </si>
   <si>
     <t>field</t>
+  </si>
+  <si>
+    <t>dateModified</t>
   </si>
 </sst>
 </file>
@@ -800,10 +800,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1127,7 +1123,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B16" sqref="B16"/>
+      <selection pane="topRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1139,13 +1135,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1153,21 +1149,21 @@
         <v>0</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="35" t="s">
-        <v>87</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1175,382 +1171,382 @@
         <v>1</v>
       </c>
       <c r="B4" s="35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
-        <v>2</v>
+        <v>109</v>
       </c>
       <c r="B5" s="35" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="14" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7" s="36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B8" s="35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B9" s="37" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="38" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="19" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B15" s="36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="22" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" s="36" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="36" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="22" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="36" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B20" s="36" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B21" s="36" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="23" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B22" s="39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B23" s="40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="25" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B24" s="35" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" s="41" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B27" s="41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" s="36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" s="35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" s="42" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" s="34" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" s="36" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33" spans="1:3" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="B33" s="41" t="s">
-        <v>82</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B34" s="36" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="31" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B35" s="36" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" s="31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B36" s="41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" s="31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B37" s="41" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B38" s="43" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>